<commit_message>
Restructure backend,  register to module events
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864309CE-E1FB-EE44-BE6A-AB9DF9266A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB0D18A-820F-DE42-9ED9-62416A5926E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="1120" windowWidth="33300" windowHeight="17880" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Gestion des configurations, récupération via API, finalisation (refactor et commentaires) du système de module</t>
+  </si>
+  <si>
+    <t>UML, rapport</t>
+  </si>
+  <si>
+    <t>Installation de l'ORM Sequelize, refactor service - repository, amélioration système de modules</t>
   </si>
 </sst>
 </file>
@@ -981,10 +987,32 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>45040</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>45040</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
@@ -995,7 +1023,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30">
         <f>SUM(C2:C29)</f>
-        <v>75.5</v>
+        <v>82.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: rework some content
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F91DF3-BD25-094A-852F-B03B2AF7664D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DED468-5ECC-DE47-ABDF-3684870FB291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -181,7 +181,13 @@
 sur les idées de modules pouvant être mis en place dans le cadre du projet: timbreuse RFID</t>
   </si>
   <si>
-    <t>Retour sur la discussion avec l'entreprise et sur le travail effectué</t>
+    <t>Intégration de la DB pour la persistance des modules et authentification des utilisateurs (JWT)</t>
+  </si>
+  <si>
+    <t>Rapport</t>
+  </si>
+  <si>
+    <t>Retour sur la discussion avec l'entreprise et sur le travail effectué, conseils sur la rédaction du rapport</t>
   </si>
 </sst>
 </file>
@@ -637,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,21 +1028,57 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30">
         <f>SUM(C2:C29)</f>
-        <v>82.5</v>
+        <v>91.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C2 C29" calculatedColumn="1"/>
+    <ignoredError sqref="C2" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1049,13 +1091,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="76.5" customWidth="1"/>
+    <col min="3" max="3" width="86.5" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
   </cols>
@@ -1137,7 +1179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45042</v>
       </c>
@@ -1156,7 +1198,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update configuration via API
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DED468-5ECC-DE47-ABDF-3684870FB291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F2DACB-F720-174C-89E3-A48377A8FEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Retour sur la discussion avec l'entreprise et sur le travail effectué, conseils sur la rédaction du rapport</t>
+  </si>
+  <si>
+    <t>Travail sur l'API, édition configuration de module</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -284,6 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,8 +310,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E30" totalsRowCount="1">
-  <autoFilter ref="A1:E29" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E39" totalsRowCount="1">
+  <autoFilter ref="A1:E38" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -319,7 +323,7 @@
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
     <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C29)</totalsRowFormula>
+      <totalsRowFormula>SUM(C2:C37)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -641,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,9 +1074,62 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C30">
-        <f>SUM(C2:C29)</f>
-        <v>91.5</v>
+      <c r="A30" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f>SUM(C2:C37)</f>
+        <v>93.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enable module API docs: work on rapport
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F2DACB-F720-174C-89E3-A48377A8FEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E680190-4CFA-8342-8A48-0086FAB640C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -276,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -287,7 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1080,8 +1079,8 @@
       <c r="B30" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="6">
-        <v>2</v>
+      <c r="C30">
+        <v>3</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
@@ -1094,42 +1093,35 @@
       <c r="B31" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31">
+        <v>3</v>
+      </c>
       <c r="D31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C39">
         <f>SUM(C2:C37)</f>
-        <v>93.5</v>
+        <v>97.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
frontend: Base of config editor
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB77B8C9-4134-BA49-8A11-A3BC23D17CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC286B7-8FD2-594B-ACDC-2F1160987B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Finalisation rapport intermédiaire</t>
+  </si>
+  <si>
+    <t>Frontend: Interface config module</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -311,6 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,8 +337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E49" totalsRowCount="1">
-  <autoFilter ref="A1:E48" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E62" totalsRowCount="1">
+  <autoFilter ref="A1:E61" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -346,7 +350,7 @@
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
     <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C48)</totalsRowFormula>
+      <totalsRowFormula>SUM(C2:C61)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -668,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,14 +1342,82 @@
       <c r="A47" s="1">
         <v>45072</v>
       </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
       <c r="D47" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49">
-        <f>SUM(C2:C48)</f>
-        <v>142.5</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="6">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="C60" s="6"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <f>SUM(C2:C61)</f>
+        <v>146.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: better module card, base of visualize route
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC286B7-8FD2-594B-ACDC-2F1160987B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15811E1-8E83-D945-B76E-7B406C023274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>Frontend: Interface config module</t>
+  </si>
+  <si>
+    <t>Feedback sur le rapport intermédiaire</t>
+  </si>
+  <si>
+    <t>Frontend:Authentification, gestion des modules (activation)</t>
+  </si>
+  <si>
+    <t>Frontend: base interface edition dashboard + visualisation</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -314,7 +323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1359,65 +1367,83 @@
       <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
-      <c r="C54" s="6"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
-      <c r="C55" s="6"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
-      <c r="C56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="C57" s="6"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
-      <c r="C58" s="6"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
-      <c r="C60" s="6"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>146.5</v>
+        <v>154.5</v>
       </c>
     </row>
   </sheetData>
@@ -1434,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8274C1-D3F0-4C46-BE21-881C4CB6257C}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,8 +1573,20 @@
         <v>48</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Toasts system & reload module after import
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15811E1-8E83-D945-B76E-7B406C023274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8C4D1C-A6D5-FC48-AEDE-FC9C10F4BDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Frontend: base interface edition dashboard + visualisation</t>
+  </si>
+  <si>
+    <t>Frontend: recherche, ajout via zip, base édition des écrans, gestion des "notifications"</t>
   </si>
 </sst>
 </file>
@@ -1416,6 +1419,20 @@
         <v>61</v>
       </c>
     </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
@@ -1443,7 +1460,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>154.5</v>
+        <v>158.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: created a custom error handler
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5A2119-447F-594B-8233-512397F62A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0C3982-A4B6-1649-92A0-D84EF35ED3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -230,6 +230,10 @@
   </si>
   <si>
     <t>Frontend: recherche, ajout via zip, base édition des écrans, gestion des "notifications", modification de la config</t>
+  </si>
+  <si>
+    <t>Frontend: Correction authentification, ajout i18n, fixes &amp; refactor
+Backend: meilleure gestion des erreurs, ajout champs actif sur écran</t>
   </si>
 </sst>
 </file>
@@ -685,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,8 +1437,19 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
@@ -1460,7 +1475,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>160.5</v>
+        <v>166.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Base of grid edition on dashbord + various fixes
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0C3982-A4B6-1649-92A0-D84EF35ED3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B09AEA7-331B-8B40-8864-55253FF602D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,9 @@
   <si>
     <t>Frontend: Correction authentification, ajout i18n, fixes &amp; refactor
 Backend: meilleure gestion des erreurs, ajout champs actif sur écran</t>
+  </si>
+  <si>
+    <t>Correctifs backend + gestion de l'édition du dashboard sur frontend</t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="140" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -1445,14 +1448,25 @@
         <v>40</v>
       </c>
       <c r="C53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1">
+        <v>45096</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
@@ -1475,7 +1489,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>166.5</v>
+        <v>170.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: user controller + base edition
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255166B-D45F-4A40-AAF5-9F5A761A1FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE1DCCB-404F-5B41-A18A-5E4909214B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -239,7 +239,7 @@
     <t>Correctifs backend + gestion de l'édition du dashboard sur frontend</t>
   </si>
   <si>
-    <t xml:space="preserve">Frontend: Gestion des dashboard 
+    <t xml:space="preserve">Frontend: Gestion des dashboard, gestion users
 Backend: refactor et validation des body </t>
   </si>
 </sst>
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="140" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -1480,7 +1480,7 @@
         <v>40</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>65</v>
@@ -1504,7 +1504,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>174.5</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: backend and modules clear + add new attributes
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33865C3-85A2-574F-B8BE-A3C8034FA6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B7B30C-CBA2-FE4B-BF07-2DB143CED47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Frontend: Correctifs de bugs globaux, améliorations ux, edition dashboard</t>
+  </si>
+  <si>
+    <t>Backend: refactor global</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,7 +1507,18 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
@@ -1518,7 +1532,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: type errors on frontend
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B7B30C-CBA2-FE4B-BF07-2DB143CED47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C101C9-296B-654B-A2FC-C15365595BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -246,7 +246,7 @@
     <t>Frontend: Correctifs de bugs globaux, améliorations ux, edition dashboard</t>
   </si>
   <si>
-    <t>Backend: refactor global</t>
+    <t>Backend: refactor global, fichier statique (modules) + style frontend, corrections de bugs</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
         <v>40</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
         <v>67</v>
@@ -1532,7 +1532,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: some frontend imrovements & style
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABD7626-D38A-EC46-A51D-DE086E72C2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D3E401-2547-6A43-97EA-6658203E59F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -249,7 +249,10 @@
     <t>Backend: refactor global, fichier statique (modules) + style frontend, corrections de bugs</t>
   </si>
   <si>
-    <t>Backend: Validation des request body</t>
+    <t>Backend: Validation des request body, reset config default, fixs</t>
+  </si>
+  <si>
+    <t>Frontend: refactor</t>
   </si>
 </sst>
 </file>
@@ -706,7 +709,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1531,14 +1534,25 @@
         <v>40</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
+      <c r="A59" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
@@ -1546,7 +1560,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: refactor, better style & new inputs
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D3E401-2547-6A43-97EA-6658203E59F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A2C107-FA77-8A44-88C7-FC622F6702E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -1548,7 +1548,7 @@
         <v>40</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
         <v>69</v>
@@ -1560,7 +1560,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <f>SUM(C2:C61)</f>
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First version of rfid module
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A2C107-FA77-8A44-88C7-FC622F6702E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C9EFB5-F8D8-6E40-AFB6-DB07088473A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
+    <workbookView xWindow="3820" yWindow="2660" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Frontend: refactor</t>
+  </si>
+  <si>
+    <t>Développement du module Composal</t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -349,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E62" totalsRowCount="1">
-  <autoFilter ref="A1:E61" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E77" totalsRowCount="1">
+  <autoFilter ref="A1:E76" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -384,7 +388,7 @@
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
     <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C61)</totalsRowFormula>
+      <totalsRowFormula>SUM(C2:C76)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -706,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,11 +1559,79 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1">
+        <v>45103</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="C61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C62">
-        <f>SUM(C2:C61)</f>
+      <c r="A62" s="1"/>
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <f>SUM(C2:C76)</f>
         <v>205</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: base for a bunch of new feature + modules
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C9EFB5-F8D8-6E40-AFB6-DB07088473A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D1DB69-D8CB-E74B-AFD3-66DD5EB5B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="2660" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -255,7 +255,10 @@
     <t>Frontend: refactor</t>
   </si>
   <si>
-    <t>Développement du module Composal</t>
+    <t>Développement du module Composal, correctifs et améliorations des fonctionnalités</t>
+  </si>
+  <si>
+    <t>Docker compile plus, à fix</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -352,7 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="C44" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,7 +1406,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45082</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45082</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45084</v>
       </c>
@@ -1446,7 +1448,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45085</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>45089</v>
       </c>
@@ -1473,8 +1475,11 @@
       <c r="D53" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45096</v>
       </c>
@@ -1488,7 +1493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45097</v>
       </c>
@@ -1502,7 +1507,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>45098</v>
       </c>
@@ -1516,7 +1521,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>45099</v>
       </c>
@@ -1530,7 +1535,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>45100</v>
       </c>
@@ -1544,7 +1549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>45101</v>
       </c>
@@ -1558,81 +1563,69 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>45103</v>
       </c>
       <c r="B60" t="s">
         <v>40</v>
       </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
       <c r="D60" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
-      <c r="C61" s="6"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="C62" s="6"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
-      <c r="C63" s="6"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
-      <c r="C64" s="6"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
-      <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="C66" s="6"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
-      <c r="C67" s="6"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="C68" s="6"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
-      <c r="C69" s="6"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
-      <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="C72" s="6"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-      <c r="C73" s="6"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
-      <c r="C74" s="6"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
-      <c r="C75" s="6"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: reset config + retrive config from db on startup
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D1DB69-D8CB-E74B-AFD3-66DD5EB5B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE98722-B983-0B45-B5E9-E61BF0FF1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="2660" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Docker compile plus, à fix</t>
+  </si>
+  <si>
+    <t>Frontend: Refactor et fonctionnalités de personnalisation</t>
+  </si>
+  <si>
+    <t>Frontend: Correctifs</t>
   </si>
 </sst>
 </file>
@@ -714,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1578,10 +1584,29 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
+      <c r="A61" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
+      <c r="A62" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
@@ -1625,7 +1650,7 @@
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: well needed rewrite and separation of concerns in Modules API routes
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE98722-B983-0B45-B5E9-E61BF0FF1F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A859B-4523-5241-BF36-A2F7518133C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="2660" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Backend: refactor global, fichier statique (modules) + style frontend, corrections de bugs</t>
   </si>
   <si>
-    <t>Backend: Validation des request body, reset config default, fixs</t>
-  </si>
-  <si>
     <t>Frontend: refactor</t>
   </si>
   <si>
@@ -264,7 +261,11 @@
     <t>Frontend: Refactor et fonctionnalités de personnalisation</t>
   </si>
   <si>
-    <t>Frontend: Correctifs</t>
+    <t>Frontend: Correctifs. Reset config + chargement de la configuration en db lors du démarrage de l'app. 
+Gestion des erreurs d'éxécution des modules (manager) et traitement des réponses (backend)</t>
+  </si>
+  <si>
+    <t>Backend: Validation des request body, reset config default, fixes</t>
   </si>
 </sst>
 </file>
@@ -721,7 +722,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,7 +1483,7 @@
         <v>63</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1552,7 +1553,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1566,7 +1567,7 @@
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1580,7 +1581,7 @@
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1594,22 +1595,30 @@
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>45105</v>
       </c>
       <c r="B62" t="s">
         <v>40</v>
       </c>
-      <c r="D62" t="s">
-        <v>73</v>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -1650,7 +1659,7 @@
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: user & auth wip
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A859B-4523-5241-BF36-A2F7518133C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB0F07B-0A47-A84D-BC81-3211D8001C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -261,11 +261,12 @@
     <t>Frontend: Refactor et fonctionnalités de personnalisation</t>
   </si>
   <si>
+    <t>Backend: Validation des request body, reset config default, fixes</t>
+  </si>
+  <si>
     <t>Frontend: Correctifs. Reset config + chargement de la configuration en db lors du démarrage de l'app. 
-Gestion des erreurs d'éxécution des modules (manager) et traitement des réponses (backend)</t>
-  </si>
-  <si>
-    <t>Backend: Validation des request body, reset config default, fixes</t>
+Gestion des erreurs d'éxécution des modules (manager) et traitement des réponses (backend)
+Refactor complet des controller - services - repos</t>
   </si>
 </sst>
 </file>
@@ -721,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1598,7 +1599,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>45105</v>
       </c>
@@ -1606,10 +1607,10 @@
         <v>40</v>
       </c>
       <c r="C62">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1659,7 +1660,7 @@
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: live sync screen update to visualize
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB0F07B-0A47-A84D-BC81-3211D8001C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3702EA-3518-7042-83D8-4F78BF72AB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,9 @@
     <t>Frontend: Correctifs. Reset config + chargement de la configuration en db lors du démarrage de l'app. 
 Gestion des erreurs d'éxécution des modules (manager) et traitement des réponses (backend)
 Refactor complet des controller - services - repos</t>
+  </si>
+  <si>
+    <t>Finalisation du refactor, mise à jour en live des écrans</t>
   </si>
 </sst>
 </file>
@@ -722,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B66" activeCellId="1" sqref="B64 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,9 +1623,20 @@
       <c r="B63" t="s">
         <v>40</v>
       </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B64" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
@@ -1660,7 +1674,7 @@
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: rewrite screen live with WS
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E73A399-C0BD-1740-97BC-6095979FB441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA37D164-8B29-7A44-880A-82C9C5BE818B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -278,7 +278,10 @@
     <t>Permet de corriger les problèmes de connexion max + memory leaks</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Refactor</t>
+  </si>
+  <si>
+    <t>Réécriture des flux live des écrans avec websockets</t>
   </si>
 </sst>
 </file>
@@ -735,7 +738,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1671,7 +1674,18 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="1">
+        <v>45110</v>
+      </c>
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
@@ -1703,7 +1717,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: a few improvements on frontend
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA37D164-8B29-7A44-880A-82C9C5BE818B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FE7EE6-1C64-EE4C-8B12-A9A79E3B6528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -281,7 +281,7 @@
     <t>Refactor</t>
   </si>
   <si>
-    <t>Réécriture des flux live des écrans avec websockets</t>
+    <t>Réécriture des flux live des écrans avec websockets, activation module live</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,14 +1681,16 @@
         <v>40</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
+      <c r="A67" s="1">
+        <v>45111</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
@@ -1717,7 +1719,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: fix docker ?
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FE7EE6-1C64-EE4C-8B12-A9A79E3B6528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E936D52-27AB-8D4E-B25A-40FE65409942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>Réécriture des flux live des écrans avec websockets, activation module live</t>
+  </si>
+  <si>
+    <t>Correction docker et test en production, mise à jour infos box (api)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +741,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,9 +1694,23 @@
       <c r="A67" s="1">
         <v>45111</v>
       </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
+      <c r="A68" s="1">
+        <v>45112</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
@@ -1719,7 +1736,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: various improves & refactor
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E936D52-27AB-8D4E-B25A-40FE65409942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18643DF7-84AE-7F4E-954F-8BAD0E7ED4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Correction docker et test en production, mise à jour infos box (api)</t>
+  </si>
+  <si>
+    <t>Correctifs, refactor, amélioration design, tests d'utilisation. Module Composal</t>
   </si>
 </sst>
 </file>
@@ -740,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1711,9 +1714,17 @@
       <c r="B68" t="s">
         <v>40</v>
       </c>
+      <c r="C68">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1">
+        <v>45113</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
@@ -1736,7 +1747,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display accessors on module page
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18643DF7-84AE-7F4E-954F-8BAD0E7ED4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97CE0D2-D360-D04A-A055-E9D413BF5DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Correctifs, refactor, amélioration design, tests d'utilisation. Module Composal</t>
+  </si>
+  <si>
+    <t>Ajout du système central d'accès audevice (accessors) et gestion des accès selon la configuration. KeyboardAccessor</t>
   </si>
 </sst>
 </file>
@@ -743,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1659,7 @@
         <v>40</v>
       </c>
       <c r="C64">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
         <v>75</v>
@@ -1673,7 +1676,7 @@
         <v>40</v>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D65" t="s">
         <v>77</v>
@@ -1725,6 +1728,15 @@
       <c r="A69" s="1">
         <v>45113</v>
       </c>
+      <c r="B69" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
@@ -1747,7 +1759,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: wip api keys, style & fixes
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97CE0D2-D360-D04A-A055-E9D413BF5DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D22B9C-0450-B642-BB24-7F0B6051E3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Ajout du système central d'accès audevice (accessors) et gestion des accès selon la configuration. KeyboardAccessor</t>
+  </si>
+  <si>
+    <t>Temps plein:</t>
+  </si>
+  <si>
+    <t>Refactor, accessor HTTP pour recevoir des des données de l'API. Début d'implémentation clés API</t>
   </si>
 </sst>
 </file>
@@ -744,17 +750,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="140" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="102.33203125" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1739,7 +1746,18 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1">
+        <v>45114</v>
+      </c>
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
@@ -1759,7 +1777,16 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>274</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79">
+        <f>SUM(C54:C75)</f>
+        <v>114.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ref: only use http accessor to receive from API, not to send
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D22B9C-0450-B642-BB24-7F0B6051E3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D67C2A-057A-944E-A332-44BFD82F7607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Refactor, accessor HTTP pour recevoir des des données de l'API. Début d'implémentation clés API</t>
+  </si>
+  <si>
+    <t>Authentification par API keys pour l'envoi vers les modules</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1498,7 @@
         <v>40</v>
       </c>
       <c r="C52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
         <v>62</v>
@@ -1540,7 +1543,7 @@
         <v>40</v>
       </c>
       <c r="C55">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>65</v>
@@ -1582,7 +1585,7 @@
         <v>40</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
         <v>72</v>
@@ -1760,7 +1763,18 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
+      <c r="A71" s="1">
+        <v>45117</v>
+      </c>
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
@@ -1777,7 +1791,7 @@
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77">
         <f>SUM(C2:C76)</f>
-        <v>282</v>
+        <v>293.5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1786,7 +1800,7 @@
       </c>
       <c r="D79">
         <f>SUM(C54:C75)</f>
-        <v>114.5</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: config validation with json shema
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D67C2A-057A-944E-A332-44BFD82F7607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ED718F-02BA-A04F-A99C-E1303F7E8E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>Authentification par API keys pour l'envoi vers les modules</t>
+  </si>
+  <si>
+    <t>Rapport: plan et idées</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation JSON schéma, </t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -396,6 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,8 +428,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E77" totalsRowCount="1">
-  <autoFilter ref="A1:E76" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E88" totalsRowCount="1">
+  <autoFilter ref="A1:E87" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -431,7 +441,7 @@
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
     <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C76)</totalsRowFormula>
+      <totalsRowFormula>SUM(C2:C87)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -753,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1777,30 +1787,107 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
+      <c r="A73" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1">
+        <v>45119</v>
+      </c>
+      <c r="B74" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="C76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C77">
-        <f>SUM(C2:C76)</f>
-        <v>293.5</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="C78" s="6"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
+      <c r="A79" s="1"/>
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <f>SUM(C2:C87)</f>
+        <v>301.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>82</v>
       </c>
-      <c r="D79">
-        <f>SUM(C54:C75)</f>
-        <v>125</v>
+      <c r="D90">
+        <f>SUM(C54:C86)</f>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few fixes & style improve on composal module
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ED718F-02BA-A04F-A99C-E1303F7E8E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D7916D-773C-4E47-B170-93903ECFCCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" activeTab="1" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -308,7 +308,13 @@
     <t>Debug</t>
   </si>
   <si>
-    <t xml:space="preserve">Validation JSON schéma, </t>
+    <t>Validation JSON schéma, correctifs, amélioration style module composal</t>
+  </si>
+  <si>
+    <t>Semestre</t>
+  </si>
+  <si>
+    <t>Discussion et démo</t>
   </si>
 </sst>
 </file>
@@ -345,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -390,11 +396,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -405,7 +422,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView topLeftCell="A67" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1452,7 +1473,7 @@
         <v>40</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D48" t="s">
         <v>58</v>
@@ -1514,24 +1535,24 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
         <v>45089</v>
       </c>
-      <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53">
+      <c r="B53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="7">
         <v>7</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45096</v>
       </c>
@@ -1822,7 +1843,7 @@
         <v>40</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D74" t="s">
         <v>87</v>
@@ -1830,47 +1851,36 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
-      <c r="C75" s="6"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
-      <c r="C76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
-      <c r="C77" s="6"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
-      <c r="C78" s="6"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
-      <c r="C79" s="6"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
-      <c r="C80" s="6"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
-      <c r="C81" s="6"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
-      <c r="C82" s="6"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
-      <c r="C83" s="6"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
-      <c r="C84" s="6"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
-      <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
@@ -1878,7 +1888,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88">
         <f>SUM(C2:C87)</f>
-        <v>301.5</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1887,7 +1897,16 @@
       </c>
       <c r="D90">
         <f>SUM(C54:C86)</f>
-        <v>133</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91">
+        <f>Tableau1[[#Totals],[Temps '[h']]] - D90</f>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1904,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8274C1-D3F0-4C46-BE21-881C4CB6257C}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,6 +2047,17 @@
         <v>59</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45119</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
docs: first batch of tb report
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E280F12-8230-DA4E-9E9D-F7C19ED32C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F366DC8-35EF-7346-A7D4-6F126E66F55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>Correction de bugs</t>
+  </si>
+  <si>
+    <t>Correction de bugs, doc swagger, feature d'envoie d'event à plusieurs modules</t>
+  </si>
+  <si>
+    <t>Structure du rapport, modules et validation</t>
   </si>
 </sst>
 </file>
@@ -804,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1944,8 +1950,11 @@
       <c r="B80" t="s">
         <v>40</v>
       </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1955,6 +1964,12 @@
       <c r="B81" t="s">
         <v>20</v>
       </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
@@ -1974,7 +1989,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88">
         <f>SUM(C2:C87)</f>
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1983,7 +1998,7 @@
       </c>
       <c r="D90">
         <f>SUM(C54:C86)</f>
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
small ref & docs
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F366DC8-35EF-7346-A7D4-6F126E66F55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8342EC-9540-DF42-8541-B02E4C266F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
+    <workbookView xWindow="2880" yWindow="1700" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Structure du rapport, modules et validation</t>
+  </si>
+  <si>
+    <t>Correctifs, doc swagger, traductions</t>
   </si>
 </sst>
 </file>
@@ -810,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1972,10 +1975,29 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="1"/>
+      <c r="A82" s="1">
+        <v>45126</v>
+      </c>
+      <c r="B82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1">
+        <v>45126</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
@@ -1989,7 +2011,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88">
         <f>SUM(C2:C87)</f>
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -1998,7 +2020,7 @@
       </c>
       <c r="D90">
         <f>SUM(C54:C86)</f>
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
docs: work on report
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1147B3-3080-8F49-ADA1-FABF878D5A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C71DB93-F6A4-F54E-97C1-4DE4C899A49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="1700" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Correctifs, doc swagger, traductions</t>
+  </si>
+  <si>
+    <t>Quelques correctif et traductions</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -454,6 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,8 +480,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E88" totalsRowCount="1">
-  <autoFilter ref="A1:E87" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E95" totalsRowCount="1">
+  <autoFilter ref="A1:E94" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -489,7 +493,7 @@
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
     <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C87)</totalsRowFormula>
+      <totalsRowFormula>SUM(C2:C94)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -811,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,6 +2013,12 @@
       <c r="B84" t="s">
         <v>40</v>
       </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2017,34 +2027,65 @@
       <c r="B85" t="s">
         <v>20</v>
       </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
       <c r="D85" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
+      <c r="C86" s="9"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C88">
-        <f>SUM(C2:C87)</f>
-        <v>348</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="C88" s="9"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
+      <c r="A90" s="1"/>
+      <c r="C90" s="9"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="C91" s="9"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="C92" s="9"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <f>SUM(C2:C94)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
         <v>82</v>
       </c>
-      <c r="D90">
-        <f>SUM(C54:C86)</f>
-        <v>179</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
+      <c r="D97">
+        <f>SUM(C54:C94)</f>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
         <v>88</v>
       </c>
-      <c r="D91">
-        <f>Tableau1[[#Totals],[Temps '[h']]] - D90</f>
+      <c r="D98">
+        <f>Tableau1[[#Totals],[Temps '[h']]] - D97</f>
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small refactor & docs
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C71DB93-F6A4-F54E-97C1-4DE4C899A49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099E9AAE-6274-304D-9F1B-852CEAD020E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="1700" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -441,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -457,7 +457,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,7 +817,7 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2035,32 +2034,36 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="1">
+        <v>45128</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
-      <c r="C87" s="9"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
-      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
-      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
-      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
-      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
-      <c r="C92" s="9"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
@@ -2068,7 +2071,7 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95">
         <f>SUM(C2:C94)</f>
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.2">
@@ -2077,7 +2080,7 @@
       </c>
       <c r="D97">
         <f>SUM(C54:C94)</f>
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
docs: content of report done
</commit_message>
<xml_diff>
--- a/docs/Journal de travail.xlsx
+++ b/docs/Journal de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Documents/_dev/TB/tb-modular-application-monorepo/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C542B710-6CCF-E748-B3E0-38EEACE4315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C0B85B-85EC-1146-882A-52FD7B28F9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{40B87E76-BD88-064F-BE2D-E0D1FA8481A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -174,9 +174,6 @@
     <t>UML, rapport</t>
   </si>
   <si>
-    <t>Installation de l'ORM Sequelize, refactor service - repository, amélioration système de modules</t>
-  </si>
-  <si>
     <t>Présentation du travail effectué, discussion 
 sur les idées de modules pouvant être mis en place dans le cadre du projet: timbreuse RFID</t>
   </si>
@@ -351,6 +348,15 @@
   </si>
   <si>
     <t>Finalisation du rapport</t>
+  </si>
+  <si>
+    <t>Etape</t>
+  </si>
+  <si>
+    <t>Refactor service - repository, amélioration système de modules</t>
+  </si>
+  <si>
+    <t>estimé</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -463,11 +469,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -485,20 +496,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:E96" totalsRowCount="1">
-  <autoFilter ref="A1:E95" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}" name="Tableau1" displayName="Tableau1" ref="A1:F96" totalsRowCount="1">
+  <autoFilter ref="A1:F95" xr:uid="{8CB6C83E-29CB-1A48-BFBE-C818E999FBE6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3EDB228-EED9-FD47-AD99-21615033BA6B}" name="Date"/>
+    <tableColumn id="6" xr3:uid="{D6172886-0EB6-0D43-8A14-6270F70F6C4C}" name="Etape" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{80555795-61E0-D443-B198-1DA7D8976B5D}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{E9B936A9-7D7D-6A47-BA5E-ADB51242CEFF}" name="Temps [h]" totalsRowFunction="custom" dataDxfId="1">
       <calculatedColumnFormula array="1">Somm</calculatedColumnFormula>
-      <totalsRowFormula>SUM(C2:C95)</totalsRowFormula>
+      <totalsRowFormula>SUM(D2:D95)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3AB59612-43D0-7444-8966-DD3CE4E87512}" name="Travail effectué"/>
     <tableColumn id="5" xr3:uid="{3625C555-138A-2B40-90A9-D72C89C957AC}" name="Commentaires"/>
@@ -820,1348 +833,1645 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A83BEE-015D-6B46-85FF-17D03AF7A340}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="102.33203125" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="102.33203125" customWidth="1"/>
+    <col min="6" max="6" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44977</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
         <v>0.5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44977</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44980</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44984</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>0.5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44984</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44990</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44991</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44991</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44998</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45001</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45012</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45019</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="9">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
         <v>0.5</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45019</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45022</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="9">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45023</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45027</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="9">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45029</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45030</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="9">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45033</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="9">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45033</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="9">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>45035</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="9">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>45036</v>
       </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="9">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
         <v>42</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>45036</v>
       </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="9">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>45040</v>
       </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="9">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25">
         <v>3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>45040</v>
       </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="9">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>45047</v>
       </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="9">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27">
         <v>6</v>
       </c>
-      <c r="D27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>45047</v>
       </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="9">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45047</v>
       </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="9">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>45050</v>
       </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="9">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30">
         <v>3</v>
       </c>
-      <c r="D30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>45050</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="9">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31">
         <v>3</v>
       </c>
-      <c r="D31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>45051</v>
       </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="9">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45051</v>
       </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="9">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33">
         <v>1.5</v>
       </c>
-      <c r="D33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45054</v>
       </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="9">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45056</v>
       </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="9">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45057</v>
       </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="9">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="D36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45058</v>
       </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="9">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45061</v>
       </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38">
+      <c r="B38" s="9">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38">
         <v>4</v>
       </c>
-      <c r="D38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45061</v>
       </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39">
+      <c r="B39" s="9">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39">
         <v>3</v>
       </c>
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45067</v>
       </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40">
+      <c r="B40" s="9">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40">
         <v>3</v>
       </c>
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45068</v>
       </c>
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="9">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41">
         <v>3</v>
       </c>
-      <c r="D41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45068</v>
       </c>
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="9">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42">
         <v>4</v>
       </c>
-      <c r="D42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45069</v>
       </c>
-      <c r="B43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="9">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43">
         <v>4</v>
       </c>
-      <c r="D43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45070</v>
       </c>
-      <c r="B44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="9">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44">
         <v>3</v>
       </c>
-      <c r="D44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45071</v>
       </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="9">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45">
         <v>4</v>
       </c>
-      <c r="D45" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45071</v>
       </c>
-      <c r="B46" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="9">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45072</v>
       </c>
-      <c r="B47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47">
+      <c r="B47" s="9">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47">
         <v>3</v>
       </c>
-      <c r="D47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45076</v>
       </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="9">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="D48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45082</v>
       </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49">
+      <c r="B49" s="9">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45082</v>
       </c>
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50">
+      <c r="B50" s="9">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
         <v>1</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45084</v>
       </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="9">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45085</v>
       </c>
-      <c r="B52" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52">
-        <v>7</v>
-      </c>
-      <c r="D52" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="9">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>45089</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="7">
-        <v>7</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="10">
+        <v>7</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="7">
+        <v>7</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45096</v>
       </c>
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="9">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54">
         <v>6</v>
       </c>
-      <c r="D54" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45097</v>
       </c>
-      <c r="B55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55">
+      <c r="B55" s="9">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55">
         <v>6</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>45098</v>
       </c>
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56">
+      <c r="B56" s="9">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56">
         <v>8</v>
       </c>
-      <c r="D56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>45099</v>
       </c>
-      <c r="B57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57">
+      <c r="B57" s="9">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57">
         <v>9</v>
       </c>
-      <c r="D57" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>45100</v>
       </c>
-      <c r="B58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58">
+      <c r="B58" s="9">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58">
         <v>6</v>
       </c>
-      <c r="D58" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>45101</v>
       </c>
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59">
+      <c r="B59" s="9">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59">
         <v>4</v>
       </c>
-      <c r="D59" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>45103</v>
       </c>
-      <c r="B60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60">
+      <c r="B60" s="9">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60">
         <v>8</v>
       </c>
-      <c r="D60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>45104</v>
       </c>
-      <c r="B61" t="s">
-        <v>40</v>
-      </c>
-      <c r="C61">
+      <c r="B61" s="9">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61">
         <v>6</v>
       </c>
-      <c r="D61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>45105</v>
       </c>
-      <c r="B62" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62">
+      <c r="B62" s="9">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62">
         <v>10</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>45106</v>
       </c>
-      <c r="B63" t="s">
-        <v>40</v>
-      </c>
-      <c r="C63">
+      <c r="B63" s="9">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63">
         <v>6</v>
       </c>
-      <c r="D63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>45107</v>
       </c>
-      <c r="B64" t="s">
-        <v>40</v>
-      </c>
-      <c r="C64">
-        <v>7</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="B64" s="9">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s">
         <v>75</v>
       </c>
-      <c r="E64" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>45108</v>
       </c>
-      <c r="B65" t="s">
-        <v>40</v>
-      </c>
-      <c r="C65">
+      <c r="B65" s="9">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65">
         <v>4</v>
       </c>
-      <c r="D65" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>45110</v>
       </c>
-      <c r="B66" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66">
+      <c r="B66" s="9">
         <v>8</v>
       </c>
-      <c r="D66" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>45111</v>
       </c>
-      <c r="B67" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67">
+      <c r="B67" s="9">
         <v>8</v>
       </c>
-      <c r="D67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>45112</v>
       </c>
-      <c r="B68" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68">
-        <v>7</v>
-      </c>
-      <c r="D68" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="9">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>45113</v>
       </c>
-      <c r="B69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C69">
+      <c r="B69" s="9">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69">
         <v>5</v>
       </c>
-      <c r="D69" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>45114</v>
       </c>
-      <c r="B70" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70">
+      <c r="B70" s="9">
         <v>8</v>
       </c>
-      <c r="D70" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>45117</v>
       </c>
-      <c r="B71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C71">
+      <c r="B71" s="9">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71">
         <v>9</v>
       </c>
-      <c r="D71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>45118</v>
       </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72">
+      <c r="B72" s="9">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72">
         <v>3</v>
       </c>
-      <c r="D72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>45118</v>
       </c>
-      <c r="B73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C73">
+      <c r="B73" s="9">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73">
         <v>3</v>
       </c>
-      <c r="D73" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>45119</v>
       </c>
-      <c r="B74" t="s">
-        <v>40</v>
-      </c>
-      <c r="C74">
+      <c r="B74" s="9">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74">
         <v>8</v>
       </c>
-      <c r="D74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>45120</v>
       </c>
-      <c r="B75" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75">
+      <c r="B75" s="9">
         <v>9</v>
       </c>
-      <c r="D75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>45121</v>
       </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76">
+      <c r="B76" s="9">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76">
         <v>1</v>
       </c>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>45121</v>
       </c>
-      <c r="B77" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77">
+      <c r="B77" s="9">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77">
         <v>6</v>
       </c>
-      <c r="D77" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>45124</v>
       </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78">
+      <c r="B78" s="9">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78">
         <v>1</v>
       </c>
-      <c r="D78" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>45124</v>
       </c>
-      <c r="B79" t="s">
-        <v>40</v>
-      </c>
-      <c r="C79">
+      <c r="B79" s="9">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79">
         <v>2</v>
       </c>
-      <c r="D79" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>45125</v>
       </c>
-      <c r="B80" t="s">
-        <v>40</v>
-      </c>
-      <c r="C80">
+      <c r="B80" s="9">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80">
         <v>5</v>
       </c>
-      <c r="D80" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>45125</v>
       </c>
-      <c r="B81" t="s">
-        <v>20</v>
-      </c>
-      <c r="C81">
+      <c r="B81" s="9">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81">
         <v>4</v>
       </c>
-      <c r="D81" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>45126</v>
       </c>
-      <c r="B82" t="s">
-        <v>40</v>
-      </c>
-      <c r="C82">
+      <c r="B82" s="9">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82">
         <v>5</v>
       </c>
-      <c r="D82" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>45126</v>
       </c>
-      <c r="B83" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83">
-        <v>7</v>
-      </c>
-      <c r="D83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="9">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83">
+        <v>7</v>
+      </c>
+      <c r="E83" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>45127</v>
       </c>
-      <c r="B84" t="s">
-        <v>40</v>
-      </c>
-      <c r="C84">
+      <c r="B84" s="9">
+        <v>10</v>
+      </c>
+      <c r="C84" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84">
         <v>2</v>
       </c>
-      <c r="D84" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>45127</v>
       </c>
-      <c r="B85" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85">
+      <c r="B85" s="9">
         <v>10</v>
       </c>
-      <c r="D85" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85">
+        <v>10</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>45128</v>
       </c>
-      <c r="B86" t="s">
-        <v>20</v>
-      </c>
-      <c r="C86">
+      <c r="B86" s="9">
         <v>10</v>
       </c>
-      <c r="D86" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>10</v>
+      </c>
+      <c r="E86" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>45129</v>
       </c>
-      <c r="B87" t="s">
-        <v>20</v>
-      </c>
-      <c r="C87">
+      <c r="B87" s="9">
+        <v>10</v>
+      </c>
+      <c r="C87" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87">
         <v>3</v>
       </c>
-      <c r="D87" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>45130</v>
       </c>
-      <c r="B88" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88">
+      <c r="B88" s="9">
+        <v>10</v>
+      </c>
+      <c r="C88" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88">
         <v>9</v>
       </c>
-      <c r="D88" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>45131</v>
       </c>
-      <c r="B89" t="s">
-        <v>40</v>
-      </c>
-      <c r="C89">
+      <c r="B89" s="9">
+        <v>10</v>
+      </c>
+      <c r="C89" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89">
         <v>1</v>
       </c>
-      <c r="D89" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>45131</v>
       </c>
-      <c r="B90" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90">
+      <c r="B90" s="9">
         <v>10</v>
       </c>
-      <c r="D90" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>45132</v>
       </c>
-      <c r="B91" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B91" s="9">
+        <v>10</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91">
+        <v>10</v>
+      </c>
+      <c r="E91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>45133</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B92" s="9">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>45134</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B93" s="9">
+        <v>10</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C96">
-        <f>SUM(C2:C95)</f>
-        <v>398</v>
-      </c>
-    </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
-        <v>82</v>
-      </c>
-      <c r="D98">
-        <f>SUM(C54:C95)</f>
-        <v>224</v>
-      </c>
-    </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>88</v>
-      </c>
-      <c r="D99">
-        <f>Tableau1[[#Totals],[Temps '[h']]] - D98</f>
+      <c r="B94" s="9"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="9"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <f>SUM(D2:D95)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>81</v>
+      </c>
+      <c r="E98">
+        <f>SUM(D54:D95)</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>87</v>
+      </c>
+      <c r="E99">
+        <f>Tableau1[[#Totals],[Temps '[h']]] - E98</f>
         <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="C2" calculatedColumn="1"/>
+    <ignoredError sqref="D2" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2270,7 +2580,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2281,7 +2591,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2292,7 +2602,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2303,7 +2613,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2314,7 +2624,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>